<commit_message>
Full Test case + Issue Logs + USER GUIDE
</commit_message>
<xml_diff>
--- a/Development and Quality Assurance/Test case/Software test case.xlsx
+++ b/Development and Quality Assurance/Test case/Software test case.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\OneDrive\RnD16Bit\Development and Quality Assurance\Test case\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2aa4bbdad9a9e3fb/RnD16Bit/Development and Quality Assurance/Test case/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="23" documentId="11_033BF99CE85592D5CC55202844AA255058C47711" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E32CEBE3-22E0-474E-9E54-A61367FBAFC8}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ArduPilot" sheetId="2" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="169">
   <si>
     <t>Project Name:</t>
   </si>
@@ -306,13 +307,7 @@
     <t>Hit the 'Routing' button on the UI</t>
   </si>
   <si>
-    <t>Face regconition</t>
-  </si>
-  <si>
     <t>From the feed received, draw a blue box on any human face</t>
-  </si>
-  <si>
-    <t>Regconise human face and mark it</t>
   </si>
   <si>
     <t>Video resolution was too big</t>
@@ -642,11 +637,20 @@
   <si>
     <t>GPS Module is disconnected and drone does not accept commands</t>
   </si>
+  <si>
+    <t>Automated flight required an ideal environment</t>
+  </si>
+  <si>
+    <t>Facial recognition</t>
+  </si>
+  <si>
+    <t>Recognize human face and mark it</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -889,7 +893,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1081,9 +1085,6 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1111,14 +1112,104 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1126,107 +1217,29 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1501,30 +1514,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" style="11" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" style="11" customWidth="1"/>
-    <col min="3" max="3" width="21.6640625" style="11" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" style="11" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" style="11" customWidth="1"/>
     <col min="4" max="4" width="32" style="11" customWidth="1"/>
-    <col min="5" max="5" width="25.44140625" style="11" customWidth="1"/>
-    <col min="6" max="6" width="25.88671875" style="11" customWidth="1"/>
-    <col min="7" max="7" width="28.44140625" style="11" customWidth="1"/>
-    <col min="8" max="8" width="12.109375" style="11" customWidth="1"/>
-    <col min="9" max="9" width="23.5546875" style="11" customWidth="1"/>
-    <col min="10" max="10" width="15.88671875" style="11" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="11"/>
+    <col min="5" max="5" width="25.42578125" style="11" customWidth="1"/>
+    <col min="6" max="6" width="25.85546875" style="11" customWidth="1"/>
+    <col min="7" max="7" width="28.42578125" style="11" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" style="11" customWidth="1"/>
+    <col min="9" max="9" width="23.5703125" style="11" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" style="11" customWidth="1"/>
+    <col min="11" max="16384" width="8.85546875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="110"/>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="79"/>
       <c r="B1" s="24" t="s">
         <v>0</v>
       </c>
@@ -1543,19 +1556,19 @@
       <c r="I1" s="1"/>
       <c r="J1" s="60"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="111"/>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="80"/>
       <c r="B2" s="24" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D2" s="33" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="25" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F2" s="34"/>
       <c r="G2" s="1"/>
@@ -1563,7 +1576,7 @@
       <c r="I2" s="1"/>
       <c r="J2" s="60"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="27"/>
       <c r="B3" s="22"/>
       <c r="C3" s="21"/>
@@ -1575,52 +1588,52 @@
       <c r="I3" s="1"/>
       <c r="J3" s="21"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="112" t="s">
+      <c r="B4" s="81" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="112"/>
-      <c r="D4" s="112"/>
-      <c r="E4" s="112"/>
-      <c r="F4" s="112"/>
+      <c r="C4" s="81"/>
+      <c r="D4" s="81"/>
+      <c r="E4" s="81"/>
+      <c r="F4" s="81"/>
       <c r="G4" s="61"/>
       <c r="H4" s="61"/>
       <c r="I4" s="61"/>
       <c r="J4" s="31"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A5" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="112" t="s">
+      <c r="B5" s="81" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="112"/>
-      <c r="D5" s="112"/>
-      <c r="E5" s="112"/>
-      <c r="F5" s="112"/>
+      <c r="C5" s="81"/>
+      <c r="D5" s="81"/>
+      <c r="E5" s="81"/>
+      <c r="F5" s="81"/>
       <c r="G5" s="61"/>
       <c r="H5" s="61"/>
       <c r="I5" s="61"/>
       <c r="J5" s="31"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="29"/>
       <c r="B6" s="30"/>
       <c r="C6" s="31"/>
       <c r="D6" s="31"/>
       <c r="E6" s="31" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F6" s="31"/>
       <c r="H6" s="31"/>
       <c r="I6" s="30"/>
       <c r="J6" s="31"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -1649,564 +1662,525 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="21" customFormat="1" ht="37.799999999999997" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" s="21" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A8" s="63">
         <v>1</v>
       </c>
       <c r="B8" s="64" t="s">
+        <v>113</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="D8" s="65" t="s">
+        <v>127</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="C8" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="D8" s="65" t="s">
-        <v>129</v>
-      </c>
-      <c r="E8" s="6" t="s">
+      <c r="F8" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="G8" s="68" t="s">
         <v>117</v>
       </c>
-      <c r="F8" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="G8" s="68" t="s">
+      <c r="H8" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="H8" s="9" t="s">
-        <v>121</v>
-      </c>
       <c r="I8" s="15" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" s="21" customFormat="1" ht="37.799999999999997" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="21" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A9" s="63">
         <v>2</v>
       </c>
       <c r="B9" s="64" t="s">
+        <v>120</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="D9" s="65" t="s">
+        <v>127</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="G9" s="66" t="s">
         <v>122</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="H9" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="D9" s="65" t="s">
+      <c r="I9" s="15" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="84">
+        <v>3</v>
+      </c>
+      <c r="B10" s="82" t="s">
+        <v>157</v>
+      </c>
+      <c r="C10" s="83" t="s">
+        <v>126</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F10" s="85" t="s">
+        <v>116</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="H10" s="88" t="s">
+        <v>119</v>
+      </c>
+      <c r="I10" s="86" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="84"/>
+      <c r="B11" s="82"/>
+      <c r="C11" s="83"/>
+      <c r="D11" s="51" t="s">
         <v>129</v>
       </c>
-      <c r="E9" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="F9" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="G9" s="66" t="s">
-        <v>124</v>
-      </c>
-      <c r="H9" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="I9" s="15" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="108">
-        <v>3</v>
-      </c>
-      <c r="B10" s="88" t="s">
+      <c r="E11" s="77" t="s">
+        <v>130</v>
+      </c>
+      <c r="F11" s="85"/>
+      <c r="G11" s="43" t="s">
+        <v>130</v>
+      </c>
+      <c r="H11" s="88"/>
+      <c r="I11" s="86"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="84"/>
+      <c r="B12" s="82"/>
+      <c r="C12" s="83"/>
+      <c r="D12" s="51" t="s">
+        <v>134</v>
+      </c>
+      <c r="E12" s="77" t="s">
+        <v>132</v>
+      </c>
+      <c r="F12" s="85"/>
+      <c r="G12" s="47" t="s">
+        <v>133</v>
+      </c>
+      <c r="H12" s="88"/>
+      <c r="I12" s="86"/>
+    </row>
+    <row r="13" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A13" s="84">
+        <v>4</v>
+      </c>
+      <c r="B13" s="82" t="s">
+        <v>157</v>
+      </c>
+      <c r="C13" s="83" t="s">
+        <v>126</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F13" s="85" t="s">
+        <v>116</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="H13" s="87" t="s">
+        <v>123</v>
+      </c>
+      <c r="I13" s="86" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="84"/>
+      <c r="B14" s="82"/>
+      <c r="C14" s="83"/>
+      <c r="D14" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="F14" s="85"/>
+      <c r="G14" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="H14" s="87"/>
+      <c r="I14" s="86"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="84"/>
+      <c r="B15" s="82"/>
+      <c r="C15" s="83"/>
+      <c r="D15" s="51" t="s">
+        <v>129</v>
+      </c>
+      <c r="E15" s="77" t="s">
+        <v>130</v>
+      </c>
+      <c r="F15" s="85"/>
+      <c r="G15" s="43" t="s">
+        <v>130</v>
+      </c>
+      <c r="H15" s="87"/>
+      <c r="I15" s="86"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="84"/>
+      <c r="B16" s="82"/>
+      <c r="C16" s="83"/>
+      <c r="D16" s="51" t="s">
+        <v>134</v>
+      </c>
+      <c r="E16" s="77" t="s">
+        <v>132</v>
+      </c>
+      <c r="F16" s="85"/>
+      <c r="G16" s="43" t="s">
+        <v>136</v>
+      </c>
+      <c r="H16" s="87"/>
+      <c r="I16" s="86"/>
+    </row>
+    <row r="17" spans="1:9" s="21" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="76">
+        <v>5</v>
+      </c>
+      <c r="B17" s="58" t="s">
+        <v>158</v>
+      </c>
+      <c r="C17" s="57" t="s">
+        <v>139</v>
+      </c>
+      <c r="D17" s="56" t="s">
+        <v>141</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="H17" s="55" t="s">
+        <v>119</v>
+      </c>
+      <c r="I17" s="56" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="76">
+        <v>6</v>
+      </c>
+      <c r="B18" s="58" t="s">
+        <v>158</v>
+      </c>
+      <c r="C18" s="57" t="s">
+        <v>144</v>
+      </c>
+      <c r="D18" s="56" t="s">
+        <v>147</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="F18" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="G18" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="H18" s="55" t="s">
+        <v>119</v>
+      </c>
+      <c r="I18" s="56" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A19" s="76">
+        <v>7</v>
+      </c>
+      <c r="B19" s="58" t="s">
+        <v>158</v>
+      </c>
+      <c r="C19" s="57" t="s">
+        <v>144</v>
+      </c>
+      <c r="D19" s="56" t="s">
+        <v>147</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="F19" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="G19" s="78" t="s">
+        <v>142</v>
+      </c>
+      <c r="H19" s="59" t="s">
+        <v>123</v>
+      </c>
+      <c r="I19" s="56"/>
+    </row>
+    <row r="20" spans="1:9" s="21" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="76">
+        <v>8</v>
+      </c>
+      <c r="B20" s="58" t="s">
+        <v>153</v>
+      </c>
+      <c r="C20" s="57" t="s">
+        <v>149</v>
+      </c>
+      <c r="D20" s="56" t="s">
+        <v>147</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="G20" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="H20" s="55" t="s">
+        <v>119</v>
+      </c>
+      <c r="I20" s="56" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" s="21" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="76">
+        <v>9</v>
+      </c>
+      <c r="B21" s="58" t="s">
+        <v>153</v>
+      </c>
+      <c r="C21" s="57" t="s">
+        <v>149</v>
+      </c>
+      <c r="D21" s="56" t="s">
+        <v>147</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="F21" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="G21" s="78" t="s">
+        <v>142</v>
+      </c>
+      <c r="H21" s="59" t="s">
+        <v>123</v>
+      </c>
+      <c r="I21" s="56" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" s="21" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="76">
+        <v>10</v>
+      </c>
+      <c r="B22" s="58" t="s">
         <v>159</v>
       </c>
-      <c r="C10" s="89" t="s">
-        <v>128</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="F10" s="81" t="s">
-        <v>118</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="H10" s="113" t="s">
-        <v>121</v>
-      </c>
-      <c r="I10" s="90" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="108"/>
-      <c r="B11" s="88"/>
-      <c r="C11" s="89"/>
-      <c r="D11" s="51" t="s">
-        <v>131</v>
-      </c>
-      <c r="E11" s="78" t="s">
-        <v>132</v>
-      </c>
-      <c r="F11" s="81"/>
-      <c r="G11" s="43" t="s">
-        <v>132</v>
-      </c>
-      <c r="H11" s="113"/>
-      <c r="I11" s="90"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="108"/>
-      <c r="B12" s="88"/>
-      <c r="C12" s="89"/>
-      <c r="D12" s="51" t="s">
-        <v>136</v>
-      </c>
-      <c r="E12" s="78" t="s">
-        <v>134</v>
-      </c>
-      <c r="F12" s="81"/>
-      <c r="G12" s="47" t="s">
-        <v>135</v>
-      </c>
-      <c r="H12" s="113"/>
-      <c r="I12" s="90"/>
-    </row>
-    <row r="13" spans="1:10" ht="37.799999999999997" x14ac:dyDescent="0.25">
-      <c r="A13" s="108">
-        <v>4</v>
-      </c>
-      <c r="B13" s="88" t="s">
+      <c r="C22" s="57" t="s">
+        <v>126</v>
+      </c>
+      <c r="D22" s="56" t="s">
+        <v>160</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="G22" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="H22" s="55" t="s">
+        <v>119</v>
+      </c>
+      <c r="I22" s="56" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" s="21" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="76">
+        <v>11</v>
+      </c>
+      <c r="B23" s="58" t="s">
         <v>159</v>
       </c>
-      <c r="C13" s="89" t="s">
-        <v>128</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="F13" s="81" t="s">
-        <v>118</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="H13" s="109" t="s">
-        <v>125</v>
-      </c>
-      <c r="I13" s="90" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="108"/>
-      <c r="B14" s="88"/>
-      <c r="C14" s="89"/>
-      <c r="D14" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="F14" s="81"/>
-      <c r="G14" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="H14" s="109"/>
-      <c r="I14" s="90"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="108"/>
-      <c r="B15" s="88"/>
-      <c r="C15" s="89"/>
-      <c r="D15" s="51" t="s">
-        <v>131</v>
-      </c>
-      <c r="E15" s="78" t="s">
-        <v>132</v>
-      </c>
-      <c r="F15" s="81"/>
-      <c r="G15" s="43" t="s">
-        <v>132</v>
-      </c>
-      <c r="H15" s="109"/>
-      <c r="I15" s="90"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="108"/>
-      <c r="B16" s="88"/>
-      <c r="C16" s="89"/>
-      <c r="D16" s="51" t="s">
-        <v>136</v>
-      </c>
-      <c r="E16" s="78" t="s">
-        <v>134</v>
-      </c>
-      <c r="F16" s="81"/>
-      <c r="G16" s="43" t="s">
-        <v>138</v>
-      </c>
-      <c r="H16" s="109"/>
-      <c r="I16" s="90"/>
-    </row>
-    <row r="17" spans="1:9" s="21" customFormat="1" ht="75.599999999999994" x14ac:dyDescent="0.3">
-      <c r="A17" s="77">
-        <v>5</v>
-      </c>
-      <c r="B17" s="58" t="s">
+      <c r="C23" s="57" t="s">
+        <v>126</v>
+      </c>
+      <c r="D23" s="56" t="s">
         <v>160</v>
       </c>
-      <c r="C17" s="57" t="s">
-        <v>141</v>
-      </c>
-      <c r="D17" s="56" t="s">
-        <v>143</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="F17" s="18" t="s">
+      <c r="E23" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="G17" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="H17" s="55" t="s">
-        <v>121</v>
-      </c>
-      <c r="I17" s="56" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="75.599999999999994" x14ac:dyDescent="0.25">
-      <c r="A18" s="77">
-        <v>6</v>
-      </c>
-      <c r="B18" s="58" t="s">
-        <v>160</v>
-      </c>
-      <c r="C18" s="57" t="s">
-        <v>146</v>
-      </c>
-      <c r="D18" s="56" t="s">
-        <v>149</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="F18" s="18" t="s">
-        <v>147</v>
-      </c>
-      <c r="G18" s="19" t="s">
-        <v>148</v>
-      </c>
-      <c r="H18" s="55" t="s">
-        <v>121</v>
-      </c>
-      <c r="I18" s="56" t="s">
+      <c r="F23" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="G23" s="19" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" ht="75.599999999999994" x14ac:dyDescent="0.25">
-      <c r="A19" s="77">
-        <v>7</v>
-      </c>
-      <c r="B19" s="58" t="s">
-        <v>160</v>
-      </c>
-      <c r="C19" s="57" t="s">
-        <v>146</v>
-      </c>
-      <c r="D19" s="56" t="s">
-        <v>149</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="F19" s="18" t="s">
-        <v>147</v>
-      </c>
-      <c r="G19" s="115" t="s">
-        <v>144</v>
-      </c>
-      <c r="H19" s="59" t="s">
-        <v>125</v>
-      </c>
-      <c r="I19" s="56"/>
-    </row>
-    <row r="20" spans="1:9" s="21" customFormat="1" ht="75.599999999999994" x14ac:dyDescent="0.3">
-      <c r="A20" s="77">
-        <v>8</v>
-      </c>
-      <c r="B20" s="58" t="s">
-        <v>155</v>
-      </c>
-      <c r="C20" s="57" t="s">
-        <v>151</v>
-      </c>
-      <c r="D20" s="56" t="s">
-        <v>149</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="F20" s="18" t="s">
-        <v>147</v>
-      </c>
-      <c r="G20" s="19" t="s">
-        <v>152</v>
-      </c>
-      <c r="H20" s="55" t="s">
-        <v>121</v>
-      </c>
-      <c r="I20" s="56" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" s="21" customFormat="1" ht="75.599999999999994" x14ac:dyDescent="0.3">
-      <c r="A21" s="77">
-        <v>9</v>
-      </c>
-      <c r="B21" s="58" t="s">
-        <v>155</v>
-      </c>
-      <c r="C21" s="57" t="s">
-        <v>151</v>
-      </c>
-      <c r="D21" s="56" t="s">
-        <v>149</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="F21" s="18" t="s">
-        <v>156</v>
-      </c>
-      <c r="G21" s="115" t="s">
-        <v>144</v>
-      </c>
-      <c r="H21" s="59" t="s">
-        <v>125</v>
-      </c>
-      <c r="I21" s="56" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" s="21" customFormat="1" ht="75.599999999999994" x14ac:dyDescent="0.3">
-      <c r="A22" s="77">
-        <v>10</v>
-      </c>
-      <c r="B22" s="58" t="s">
-        <v>161</v>
-      </c>
-      <c r="C22" s="57" t="s">
-        <v>128</v>
-      </c>
-      <c r="D22" s="56" t="s">
-        <v>162</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="F22" s="18" t="s">
-        <v>163</v>
-      </c>
-      <c r="G22" s="19" t="s">
-        <v>164</v>
-      </c>
-      <c r="H22" s="55" t="s">
-        <v>121</v>
-      </c>
-      <c r="I22" s="56" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" s="21" customFormat="1" ht="75.599999999999994" x14ac:dyDescent="0.3">
-      <c r="A23" s="77">
-        <v>11</v>
-      </c>
-      <c r="B23" s="58" t="s">
-        <v>161</v>
-      </c>
-      <c r="C23" s="57" t="s">
-        <v>128</v>
-      </c>
-      <c r="D23" s="56" t="s">
-        <v>162</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="F23" s="18" t="s">
+      <c r="H23" s="55" t="s">
+        <v>119</v>
+      </c>
+      <c r="I23" s="56" t="s">
         <v>165</v>
       </c>
-      <c r="G23" s="19" t="s">
-        <v>152</v>
-      </c>
-      <c r="H23" s="55" t="s">
-        <v>121</v>
-      </c>
-      <c r="I23" s="56" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" s="21" customFormat="1" ht="75.599999999999994" x14ac:dyDescent="0.3">
-      <c r="A24" s="114">
-        <v>12</v>
-      </c>
-      <c r="B24" s="58" t="s">
-        <v>161</v>
-      </c>
-      <c r="C24" s="57" t="s">
-        <v>128</v>
-      </c>
-      <c r="D24" s="56" t="s">
-        <v>162</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>144</v>
-      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="67"/>
+      <c r="B24" s="69"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="72"/>
       <c r="F24" s="16"/>
       <c r="G24" s="16"/>
-      <c r="H24" s="74"/>
-      <c r="I24" s="73"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="69"/>
+      <c r="H24" s="73"/>
+      <c r="I24" s="72"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="67"/>
       <c r="B25" s="70"/>
-      <c r="C25" s="16"/>
+      <c r="C25" s="74"/>
       <c r="D25" s="16"/>
-      <c r="E25" s="73"/>
+      <c r="E25" s="72"/>
       <c r="F25" s="16"/>
       <c r="G25" s="16"/>
-      <c r="H25" s="74"/>
-      <c r="I25" s="73"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H25" s="73"/>
+      <c r="I25" s="72"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="67"/>
-      <c r="B26" s="70"/>
-      <c r="C26" s="16"/>
+      <c r="B26" s="71"/>
+      <c r="C26" s="74"/>
       <c r="D26" s="16"/>
-      <c r="E26" s="73"/>
+      <c r="E26" s="72"/>
       <c r="F26" s="16"/>
       <c r="G26" s="16"/>
-      <c r="H26" s="74"/>
-      <c r="I26" s="73"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H26" s="73"/>
+      <c r="I26" s="72"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="67"/>
       <c r="B27" s="71"/>
-      <c r="C27" s="75"/>
+      <c r="C27" s="74"/>
       <c r="D27" s="16"/>
-      <c r="E27" s="73"/>
+      <c r="E27" s="72"/>
       <c r="F27" s="16"/>
       <c r="G27" s="16"/>
-      <c r="H27" s="74"/>
-      <c r="I27" s="73"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H27" s="73"/>
+      <c r="I27" s="72"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="67"/>
-      <c r="B28" s="72"/>
-      <c r="C28" s="75"/>
+      <c r="B28" s="71"/>
+      <c r="C28" s="74"/>
       <c r="D28" s="16"/>
-      <c r="E28" s="73"/>
+      <c r="E28" s="72"/>
       <c r="F28" s="16"/>
       <c r="G28" s="16"/>
-      <c r="H28" s="74"/>
-      <c r="I28" s="73"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H28" s="16"/>
+      <c r="I28" s="16"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="67"/>
-      <c r="B29" s="72"/>
-      <c r="C29" s="75"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="73"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="74"/>
-      <c r="I29" s="73"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="75"/>
+      <c r="F29" s="41"/>
+      <c r="G29" s="41"/>
+      <c r="H29" s="41"/>
+      <c r="I29" s="41"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="67"/>
-      <c r="B30" s="72"/>
-      <c r="C30" s="75"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="73"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="16"/>
-      <c r="I30" s="16"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="67"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="75"/>
+      <c r="F30" s="41"/>
+      <c r="G30" s="41"/>
+      <c r="H30" s="41"/>
+      <c r="I30" s="41"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C31" s="12"/>
       <c r="D31" s="12"/>
-      <c r="E31" s="76"/>
+      <c r="E31" s="12"/>
       <c r="F31" s="41"/>
       <c r="G31" s="41"/>
       <c r="H31" s="41"/>
       <c r="I31" s="41"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="67"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="76"/>
-      <c r="F32" s="41"/>
-      <c r="G32" s="41"/>
-      <c r="H32" s="41"/>
-      <c r="I32" s="41"/>
-    </row>
-    <row r="33" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="41"/>
-      <c r="G33" s="41"/>
-      <c r="H33" s="41"/>
-      <c r="I33" s="41"/>
-    </row>
-    <row r="34" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="F34" s="21"/>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F32" s="21"/>
+      <c r="G32" s="21"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="21"/>
+    </row>
+    <row r="33" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="F33" s="21"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="21"/>
+      <c r="I33" s="21"/>
+    </row>
+    <row r="34" spans="6:9" x14ac:dyDescent="0.2">
       <c r="G34" s="21"/>
       <c r="H34" s="21"/>
       <c r="I34" s="21"/>
     </row>
-    <row r="35" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="F35" s="21"/>
-      <c r="G35" s="21"/>
+    <row r="35" spans="6:9" x14ac:dyDescent="0.2">
       <c r="H35" s="21"/>
       <c r="I35" s="21"/>
     </row>
-    <row r="36" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="G36" s="21"/>
+    <row r="36" spans="6:9" x14ac:dyDescent="0.2">
       <c r="H36" s="21"/>
       <c r="I36" s="21"/>
     </row>
-    <row r="37" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="H37" s="21"/>
+    <row r="37" spans="6:9" x14ac:dyDescent="0.2">
       <c r="I37" s="21"/>
     </row>
-    <row r="38" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="H38" s="21"/>
+    <row r="38" spans="6:9" x14ac:dyDescent="0.2">
       <c r="I38" s="21"/>
-    </row>
-    <row r="39" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="I39" s="21"/>
-    </row>
-    <row r="40" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="I40" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="F10:F12"/>
     <mergeCell ref="I10:I12"/>
     <mergeCell ref="B13:B16"/>
     <mergeCell ref="C13:C16"/>
@@ -2215,38 +2189,53 @@
     <mergeCell ref="H13:H16"/>
     <mergeCell ref="I13:I16"/>
     <mergeCell ref="H10:H12"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="F10:F12"/>
   </mergeCells>
+  <conditionalFormatting sqref="H8:H23">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"PASS"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>"FAILED"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21:B24"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="I34" sqref="I34:I36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" style="11" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" style="11" customWidth="1"/>
-    <col min="3" max="3" width="21.6640625" style="11" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" style="11" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" style="11" customWidth="1"/>
     <col min="4" max="4" width="32" style="11" customWidth="1"/>
-    <col min="5" max="5" width="25.44140625" style="11" customWidth="1"/>
-    <col min="6" max="6" width="25.88671875" style="11" customWidth="1"/>
-    <col min="7" max="7" width="28.44140625" style="11" customWidth="1"/>
-    <col min="8" max="8" width="12.109375" style="11" customWidth="1"/>
-    <col min="9" max="9" width="23.5546875" style="11" customWidth="1"/>
-    <col min="10" max="10" width="15.88671875" style="11" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="11"/>
+    <col min="5" max="5" width="25.42578125" style="11" customWidth="1"/>
+    <col min="6" max="6" width="25.85546875" style="11" customWidth="1"/>
+    <col min="7" max="7" width="28.42578125" style="11" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" style="11" customWidth="1"/>
+    <col min="9" max="9" width="23.5703125" style="11" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" style="11" customWidth="1"/>
+    <col min="11" max="16384" width="8.85546875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="82"/>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="111"/>
       <c r="B1" s="24" t="s">
         <v>0</v>
       </c>
@@ -2265,8 +2254,8 @@
       <c r="I1" s="1"/>
       <c r="J1" s="26"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="83"/>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="112"/>
       <c r="B2" s="24" t="s">
         <v>4</v>
       </c>
@@ -2277,7 +2266,7 @@
         <v>6</v>
       </c>
       <c r="E2" s="25" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F2" s="34"/>
       <c r="G2" s="1"/>
@@ -2285,7 +2274,7 @@
       <c r="I2" s="1"/>
       <c r="J2" s="26"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="27"/>
       <c r="B3" s="22"/>
       <c r="C3" s="21"/>
@@ -2297,39 +2286,39 @@
       <c r="I3" s="1"/>
       <c r="J3" s="21"/>
     </row>
-    <row r="4" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="85" t="s">
+      <c r="B4" s="113" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="85"/>
-      <c r="D4" s="85"/>
-      <c r="E4" s="85"/>
-      <c r="F4" s="85"/>
+      <c r="C4" s="113"/>
+      <c r="D4" s="113"/>
+      <c r="E4" s="113"/>
+      <c r="F4" s="113"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="28"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="85" t="s">
+      <c r="B5" s="113" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="85"/>
-      <c r="D5" s="85"/>
-      <c r="E5" s="85"/>
-      <c r="F5" s="85"/>
+      <c r="C5" s="113"/>
+      <c r="D5" s="113"/>
+      <c r="E5" s="113"/>
+      <c r="F5" s="113"/>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" s="28"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="29"/>
       <c r="B6" s="30"/>
       <c r="C6" s="31"/>
@@ -2341,7 +2330,7 @@
       <c r="I6" s="30"/>
       <c r="J6" s="31"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -2370,14 +2359,14 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="79">
+    <row r="8" spans="1:10" ht="37.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="108">
         <v>1</v>
       </c>
-      <c r="B8" s="80" t="s">
+      <c r="B8" s="109" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="84" t="s">
+      <c r="C8" s="105" t="s">
         <v>30</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -2386,46 +2375,46 @@
       <c r="E8" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="81" t="s">
+      <c r="F8" s="85" t="s">
         <v>24</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H8" s="95" t="s">
+      <c r="H8" s="96" t="s">
         <v>20</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="35.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="79"/>
-      <c r="B9" s="80"/>
-      <c r="C9" s="84"/>
+    <row r="9" spans="1:10" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="108"/>
+      <c r="B9" s="109"/>
+      <c r="C9" s="105"/>
       <c r="D9" s="3" t="s">
         <v>28</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="81"/>
+      <c r="F9" s="85"/>
       <c r="G9" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="H9" s="96"/>
+      <c r="H9" s="97"/>
       <c r="I9" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="79">
+    <row r="10" spans="1:10" ht="29.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="108">
         <v>2</v>
       </c>
-      <c r="B10" s="80" t="s">
+      <c r="B10" s="109" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="84" t="s">
+      <c r="C10" s="105" t="s">
         <v>31</v>
       </c>
       <c r="D10" s="3" t="s">
@@ -2434,61 +2423,61 @@
       <c r="E10" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="F10" s="81" t="s">
+      <c r="F10" s="85" t="s">
         <v>24</v>
       </c>
       <c r="G10" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="H10" s="95" t="s">
+      <c r="H10" s="96" t="s">
         <v>20</v>
       </c>
-      <c r="I10" s="81" t="s">
+      <c r="I10" s="85" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="25.2" x14ac:dyDescent="0.25">
-      <c r="A11" s="79"/>
-      <c r="B11" s="80"/>
-      <c r="C11" s="84"/>
+    <row r="11" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A11" s="108"/>
+      <c r="B11" s="109"/>
+      <c r="C11" s="105"/>
       <c r="D11" s="3" t="s">
         <v>39</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F11" s="81"/>
+      <c r="F11" s="85"/>
       <c r="G11" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="H11" s="100"/>
-      <c r="I11" s="81"/>
-    </row>
-    <row r="12" spans="1:10" ht="43.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="79"/>
-      <c r="B12" s="80"/>
-      <c r="C12" s="84"/>
+      <c r="H11" s="101"/>
+      <c r="I11" s="85"/>
+    </row>
+    <row r="12" spans="1:10" ht="43.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="108"/>
+      <c r="B12" s="109"/>
+      <c r="C12" s="105"/>
       <c r="D12" s="3" t="s">
         <v>40</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="F12" s="81"/>
+      <c r="F12" s="85"/>
       <c r="G12" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="H12" s="96"/>
-      <c r="I12" s="81"/>
-    </row>
-    <row r="13" spans="1:10" ht="25.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="79">
+      <c r="H12" s="97"/>
+      <c r="I12" s="85"/>
+    </row>
+    <row r="13" spans="1:10" ht="25.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="108">
         <v>3</v>
       </c>
-      <c r="B13" s="80" t="s">
+      <c r="B13" s="109" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="84" t="s">
+      <c r="C13" s="105" t="s">
         <v>42</v>
       </c>
       <c r="D13" s="3" t="s">
@@ -2497,44 +2486,44 @@
       <c r="E13" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="F13" s="81" t="s">
+      <c r="F13" s="85" t="s">
         <v>24</v>
       </c>
       <c r="G13" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="H13" s="95" t="s">
+      <c r="H13" s="96" t="s">
         <v>20</v>
       </c>
-      <c r="I13" s="81" t="s">
+      <c r="I13" s="85" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="79"/>
-      <c r="B14" s="80"/>
-      <c r="C14" s="84"/>
+    <row r="14" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="108"/>
+      <c r="B14" s="109"/>
+      <c r="C14" s="105"/>
       <c r="D14" s="3" t="s">
         <v>44</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F14" s="81"/>
+      <c r="F14" s="85"/>
       <c r="G14" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="H14" s="96"/>
-      <c r="I14" s="81"/>
-    </row>
-    <row r="15" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="86">
+      <c r="H14" s="97"/>
+      <c r="I14" s="85"/>
+    </row>
+    <row r="15" spans="1:10" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="110">
         <v>4</v>
       </c>
-      <c r="B15" s="80" t="s">
+      <c r="B15" s="109" t="s">
         <v>49</v>
       </c>
-      <c r="C15" s="84" t="s">
+      <c r="C15" s="105" t="s">
         <v>50</v>
       </c>
       <c r="D15" s="3" t="s">
@@ -2549,57 +2538,57 @@
       <c r="G15" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="H15" s="97" t="s">
+      <c r="H15" s="98" t="s">
         <v>59</v>
       </c>
       <c r="I15" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="86"/>
-      <c r="B16" s="80"/>
-      <c r="C16" s="84"/>
+    <row r="16" spans="1:10" ht="30.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="110"/>
+      <c r="B16" s="109"/>
+      <c r="C16" s="105"/>
       <c r="D16" s="3" t="s">
         <v>53</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="F16" s="102"/>
+      <c r="F16" s="103"/>
       <c r="G16" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="H16" s="98"/>
-      <c r="I16" s="103" t="s">
+      <c r="H16" s="99"/>
+      <c r="I16" s="104" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="25.2" x14ac:dyDescent="0.25">
-      <c r="A17" s="86"/>
-      <c r="B17" s="80"/>
-      <c r="C17" s="84"/>
+    <row r="17" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A17" s="110"/>
+      <c r="B17" s="109"/>
+      <c r="C17" s="105"/>
       <c r="D17" s="3" t="s">
         <v>54</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="F17" s="102"/>
+      <c r="F17" s="103"/>
       <c r="G17" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="H17" s="99"/>
-      <c r="I17" s="81"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="79">
+      <c r="H17" s="100"/>
+      <c r="I17" s="85"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="108">
         <v>5</v>
       </c>
-      <c r="B18" s="104" t="s">
+      <c r="B18" s="106" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="84" t="s">
+      <c r="C18" s="105" t="s">
         <v>50</v>
       </c>
       <c r="D18" s="3" t="s">
@@ -2614,52 +2603,52 @@
       <c r="G18" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="H18" s="95" t="s">
+      <c r="H18" s="96" t="s">
         <v>20</v>
       </c>
       <c r="I18" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="25.2" x14ac:dyDescent="0.25">
-      <c r="A19" s="79"/>
-      <c r="B19" s="104"/>
-      <c r="C19" s="84"/>
+    <row r="19" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A19" s="108"/>
+      <c r="B19" s="106"/>
+      <c r="C19" s="105"/>
       <c r="D19" s="3" t="s">
         <v>53</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="F19" s="101" t="s">
+      <c r="F19" s="102" t="s">
         <v>62</v>
       </c>
       <c r="G19" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="H19" s="100"/>
-      <c r="I19" s="81" t="s">
+      <c r="H19" s="101"/>
+      <c r="I19" s="85" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="25.2" x14ac:dyDescent="0.25">
-      <c r="A20" s="79"/>
-      <c r="B20" s="104"/>
-      <c r="C20" s="84"/>
+    <row r="20" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A20" s="108"/>
+      <c r="B20" s="106"/>
+      <c r="C20" s="105"/>
       <c r="D20" s="3" t="s">
         <v>54</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="F20" s="101"/>
+      <c r="F20" s="102"/>
       <c r="G20" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="H20" s="96"/>
-      <c r="I20" s="81"/>
-    </row>
-    <row r="21" spans="1:10" ht="31.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H20" s="97"/>
+      <c r="I20" s="85"/>
+    </row>
+    <row r="21" spans="1:10" ht="31.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="46">
         <v>6</v>
       </c>
@@ -2718,7 +2707,7 @@
       </c>
       <c r="J22" s="44"/>
     </row>
-    <row r="23" spans="1:10" s="40" customFormat="1" ht="37.799999999999997" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" s="40" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A23" s="35">
         <v>8</v>
       </c>
@@ -2748,7 +2737,7 @@
       </c>
       <c r="J23" s="45"/>
     </row>
-    <row r="24" spans="1:10" s="41" customFormat="1" ht="37.799999999999997" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" s="41" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A24" s="35">
         <v>9</v>
       </c>
@@ -2777,7 +2766,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="25" spans="1:10" s="41" customFormat="1" ht="50.4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" s="41" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A25" s="35">
         <v>10</v>
       </c>
@@ -2803,10 +2792,10 @@
         <v>59</v>
       </c>
       <c r="I25" s="20" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" s="41" customFormat="1" ht="50.4" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" s="41" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A26" s="35">
         <v>11</v>
       </c>
@@ -2835,7 +2824,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:10" s="41" customFormat="1" ht="37.799999999999997" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" s="41" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A27" s="35">
         <v>12</v>
       </c>
@@ -2864,21 +2853,21 @@
         <v>88</v>
       </c>
     </row>
-    <row r="28" spans="1:10" s="41" customFormat="1" ht="37.799999999999997" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" s="41" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A28" s="35">
         <v>13</v>
       </c>
       <c r="B28" s="48" t="s">
+        <v>167</v>
+      </c>
+      <c r="C28" s="49" t="s">
+        <v>168</v>
+      </c>
+      <c r="D28" s="40" t="s">
+        <v>101</v>
+      </c>
+      <c r="E28" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="C28" s="49" t="s">
-        <v>95</v>
-      </c>
-      <c r="D28" s="40" t="s">
-        <v>103</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>94</v>
       </c>
       <c r="F28" s="20" t="s">
         <v>85</v>
@@ -2890,24 +2879,24 @@
         <v>59</v>
       </c>
       <c r="I28" s="20" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" s="41" customFormat="1" ht="37.799999999999997" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" s="41" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A29" s="35">
         <v>14</v>
       </c>
-      <c r="B29" s="36" t="s">
+      <c r="B29" s="48" t="s">
+        <v>167</v>
+      </c>
+      <c r="C29" s="49" t="s">
+        <v>168</v>
+      </c>
+      <c r="D29" s="40" t="s">
+        <v>101</v>
+      </c>
+      <c r="E29" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="C29" s="49" t="s">
-        <v>95</v>
-      </c>
-      <c r="D29" s="40" t="s">
-        <v>103</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>94</v>
       </c>
       <c r="F29" s="20" t="s">
         <v>85</v>
@@ -2919,53 +2908,53 @@
         <v>20</v>
       </c>
       <c r="I29" s="20" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" s="41" customFormat="1" ht="25.2" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" s="41" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A30" s="35">
         <v>15</v>
       </c>
       <c r="B30" s="52" t="s">
+        <v>96</v>
+      </c>
+      <c r="C30" s="37" t="s">
+        <v>97</v>
+      </c>
+      <c r="D30" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="E30" s="6" t="s">
         <v>98</v>
-      </c>
-      <c r="C30" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="D30" s="20" t="s">
-        <v>102</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>100</v>
       </c>
       <c r="F30" s="20" t="s">
         <v>85</v>
       </c>
       <c r="G30" s="47" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H30" s="38" t="s">
         <v>59</v>
       </c>
       <c r="I30" s="20" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" s="16" customFormat="1" ht="25.2" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" s="16" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A31" s="50">
         <v>16</v>
       </c>
       <c r="B31" s="53" t="s">
+        <v>96</v>
+      </c>
+      <c r="C31" s="37" t="s">
+        <v>97</v>
+      </c>
+      <c r="D31" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="E31" s="6" t="s">
         <v>98</v>
-      </c>
-      <c r="C31" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="D31" s="20" t="s">
-        <v>102</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>100</v>
       </c>
       <c r="F31" s="20" t="s">
         <v>85</v>
@@ -2977,192 +2966,208 @@
         <v>59</v>
       </c>
       <c r="I31" s="20" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" s="41" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="107">
+        <v>17</v>
+      </c>
+      <c r="B32" s="82" t="s">
+        <v>96</v>
+      </c>
+      <c r="C32" s="83" t="s">
+        <v>97</v>
+      </c>
+      <c r="D32" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="E32" s="54" t="s">
+        <v>98</v>
+      </c>
+      <c r="F32" s="86" t="s">
+        <v>85</v>
+      </c>
+      <c r="G32" s="43" t="s">
+        <v>103</v>
+      </c>
+      <c r="H32" s="90" t="s">
+        <v>59</v>
+      </c>
+      <c r="I32" s="93" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" s="41" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A33" s="107"/>
+      <c r="B33" s="82"/>
+      <c r="C33" s="83"/>
+      <c r="D33" s="18" t="s">
         <v>107</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" s="41" customFormat="1" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="87">
-        <v>17</v>
-      </c>
-      <c r="B32" s="88" t="s">
-        <v>98</v>
-      </c>
-      <c r="C32" s="89" t="s">
-        <v>99</v>
-      </c>
-      <c r="D32" s="18" t="s">
-        <v>102</v>
-      </c>
-      <c r="E32" s="54" t="s">
-        <v>100</v>
-      </c>
-      <c r="F32" s="90" t="s">
-        <v>85</v>
-      </c>
-      <c r="G32" s="43" t="s">
-        <v>105</v>
-      </c>
-      <c r="H32" s="91" t="s">
-        <v>59</v>
-      </c>
-      <c r="I32" s="92" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" s="41" customFormat="1" ht="25.2" x14ac:dyDescent="0.3">
-      <c r="A33" s="87"/>
-      <c r="B33" s="88"/>
-      <c r="C33" s="89"/>
-      <c r="D33" s="18" t="s">
-        <v>109</v>
       </c>
       <c r="E33" s="54" t="s">
         <v>68</v>
       </c>
-      <c r="F33" s="90"/>
+      <c r="F33" s="86"/>
       <c r="G33" s="47" t="s">
         <v>86</v>
       </c>
-      <c r="H33" s="91"/>
-      <c r="I33" s="93"/>
-    </row>
-    <row r="34" spans="1:9" s="41" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="105">
+      <c r="H33" s="90"/>
+      <c r="I33" s="94"/>
+    </row>
+    <row r="34" spans="1:9" s="41" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="89">
         <v>18</v>
       </c>
-      <c r="B34" s="94" t="s">
+      <c r="B34" s="95" t="s">
+        <v>96</v>
+      </c>
+      <c r="C34" s="83" t="s">
+        <v>97</v>
+      </c>
+      <c r="D34" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="E34" s="54" t="s">
         <v>98</v>
       </c>
-      <c r="C34" s="89" t="s">
-        <v>99</v>
-      </c>
-      <c r="D34" s="18" t="s">
-        <v>102</v>
-      </c>
-      <c r="E34" s="54" t="s">
-        <v>100</v>
-      </c>
-      <c r="F34" s="90" t="s">
+      <c r="F34" s="86" t="s">
         <v>85</v>
       </c>
       <c r="G34" s="43" t="s">
-        <v>105</v>
-      </c>
-      <c r="H34" s="91" t="s">
+        <v>103</v>
+      </c>
+      <c r="H34" s="90" t="s">
         <v>59</v>
       </c>
-      <c r="I34" s="90" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" s="41" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="105"/>
-      <c r="B35" s="94"/>
-      <c r="C35" s="89"/>
+      <c r="I34" s="86" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" s="41" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="89"/>
+      <c r="B35" s="95"/>
+      <c r="C35" s="83"/>
       <c r="D35" s="18" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E35" s="54" t="s">
         <v>68</v>
       </c>
-      <c r="F35" s="90"/>
+      <c r="F35" s="86"/>
       <c r="G35" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="H35" s="91"/>
-      <c r="I35" s="90"/>
-    </row>
-    <row r="36" spans="1:9" s="41" customFormat="1" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="105"/>
-      <c r="B36" s="94"/>
-      <c r="C36" s="89"/>
+      <c r="H35" s="90"/>
+      <c r="I35" s="86"/>
+    </row>
+    <row r="36" spans="1:9" s="41" customFormat="1" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="89"/>
+      <c r="B36" s="95"/>
+      <c r="C36" s="83"/>
       <c r="D36" s="39" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E36" s="54" t="s">
         <v>68</v>
       </c>
-      <c r="F36" s="90"/>
+      <c r="F36" s="86"/>
       <c r="G36" s="47" t="s">
+        <v>110</v>
+      </c>
+      <c r="H36" s="90"/>
+      <c r="I36" s="86"/>
+    </row>
+    <row r="37" spans="1:9" s="41" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="89">
+        <v>19</v>
+      </c>
+      <c r="B37" s="82" t="s">
+        <v>96</v>
+      </c>
+      <c r="C37" s="83" t="s">
+        <v>97</v>
+      </c>
+      <c r="D37" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="E37" s="54" t="s">
+        <v>98</v>
+      </c>
+      <c r="F37" s="86" t="s">
+        <v>85</v>
+      </c>
+      <c r="G37" s="43" t="s">
+        <v>103</v>
+      </c>
+      <c r="H37" s="91" t="s">
+        <v>20</v>
+      </c>
+      <c r="I37" s="92" t="s">
         <v>112</v>
       </c>
-      <c r="H36" s="91"/>
-      <c r="I36" s="90"/>
-    </row>
-    <row r="37" spans="1:9" s="41" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="105">
-        <v>19</v>
-      </c>
-      <c r="B37" s="88" t="s">
-        <v>98</v>
-      </c>
-      <c r="C37" s="89" t="s">
-        <v>99</v>
-      </c>
-      <c r="D37" s="18" t="s">
-        <v>102</v>
-      </c>
-      <c r="E37" s="54" t="s">
-        <v>100</v>
-      </c>
-      <c r="F37" s="90" t="s">
-        <v>85</v>
-      </c>
-      <c r="G37" s="43" t="s">
-        <v>105</v>
-      </c>
-      <c r="H37" s="106" t="s">
-        <v>20</v>
-      </c>
-      <c r="I37" s="107" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" s="12" customFormat="1" ht="16.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="105"/>
-      <c r="B38" s="88"/>
-      <c r="C38" s="89"/>
+    </row>
+    <row r="38" spans="1:9" s="12" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="89"/>
+      <c r="B38" s="82"/>
+      <c r="C38" s="83"/>
       <c r="D38" s="18" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E38" s="54" t="s">
         <v>68</v>
       </c>
-      <c r="F38" s="90"/>
+      <c r="F38" s="86"/>
       <c r="G38" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="H38" s="106"/>
-      <c r="I38" s="107"/>
-    </row>
-    <row r="39" spans="1:9" ht="16.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="105"/>
-      <c r="B39" s="88"/>
-      <c r="C39" s="89"/>
+      <c r="H38" s="91"/>
+      <c r="I38" s="92"/>
+    </row>
+    <row r="39" spans="1:9" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="89"/>
+      <c r="B39" s="82"/>
+      <c r="C39" s="83"/>
       <c r="D39" s="39" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E39" s="54" t="s">
         <v>68</v>
       </c>
-      <c r="F39" s="90"/>
+      <c r="F39" s="86"/>
       <c r="G39" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="H39" s="106"/>
-      <c r="I39" s="107"/>
+      <c r="H39" s="91"/>
+      <c r="I39" s="92"/>
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="H34:H36"/>
-    <mergeCell ref="I34:I36"/>
-    <mergeCell ref="C37:C39"/>
-    <mergeCell ref="B37:B39"/>
-    <mergeCell ref="A37:A39"/>
-    <mergeCell ref="F37:F39"/>
-    <mergeCell ref="H37:H39"/>
-    <mergeCell ref="I37:I39"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="I10:I12"/>
+    <mergeCell ref="F10:F12"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="H32:H33"/>
     <mergeCell ref="I32:I33"/>
     <mergeCell ref="F34:F36"/>
     <mergeCell ref="C34:C36"/>
@@ -3179,31 +3184,15 @@
     <mergeCell ref="C18:C20"/>
     <mergeCell ref="B18:B20"/>
     <mergeCell ref="C10:C12"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="F32:F33"/>
-    <mergeCell ref="H32:H33"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="I10:I12"/>
-    <mergeCell ref="F10:F12"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="H34:H36"/>
+    <mergeCell ref="I34:I36"/>
+    <mergeCell ref="C37:C39"/>
+    <mergeCell ref="B37:B39"/>
+    <mergeCell ref="A37:A39"/>
+    <mergeCell ref="F37:F39"/>
+    <mergeCell ref="H37:H39"/>
+    <mergeCell ref="I37:I39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>